<commit_message>
ret more info on del objects
</commit_message>
<xml_diff>
--- a/zootable/test_data/example.xlsx
+++ b/zootable/test_data/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t xml:space="preserve">Enclosure</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t xml:space="preserve">species2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a square nose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a yellow nose</t>
   </si>
 </sst>
 </file>
@@ -217,10 +229,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,6 +387,98 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1111113</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1111114</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
convert accession nums to char
ignore case on default ordering

validate that all accession numbers are 6 digits
</commit_message>
<xml_diff>
--- a/zootable/test_data/example.xlsx
+++ b/zootable/test_data/example.xlsx
@@ -257,15 +257,13 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,7 +327,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1111111</v>
+        <v>111111</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
@@ -375,7 +373,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1111112</v>
+        <v>111112</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>27</v>
@@ -417,7 +415,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>1111113</v>
+        <v>111113</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -463,7 +461,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>1111114</v>
+        <v>111114</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>27</v>

</xml_diff>